<commit_message>
PMD - UseStringBufferLength specified
</commit_message>
<xml_diff>
--- a/pmd-rules-transformation-progress.xlsx
+++ b/pmd-rules-transformation-progress.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git-repositories\Coding-Conventions-Specification-Language\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CF16A21-2441-4E12-86AB-DCAD6F2D0C9D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2BC9795-DCDA-4A03-B6AF-DBF06FC71238}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -478,17 +478,17 @@
   <dimension ref="A1:E31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="50.109375" customWidth="1"/>
-    <col min="3" max="3" width="28.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.33203125" customWidth="1"/>
+    <col min="1" max="1" width="50.140625" customWidth="1"/>
+    <col min="3" max="3" width="28.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -499,7 +499,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -511,14 +511,14 @@
       </c>
       <c r="D2" s="2">
         <f>COUNTIF(B2:B31, "ok")</f>
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E2">
         <f xml:space="preserve"> (D2 / D1) * 100</f>
-        <v>73.333333333333329</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+        <v>76.666666666666671</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -537,7 +537,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -549,14 +549,14 @@
       </c>
       <c r="D4" s="2">
         <f>COUNTIF(B4:B33, "later")</f>
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E4">
         <f xml:space="preserve"> (D4 / D1) * 100</f>
-        <v>26.666666666666668</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+        <v>23.333333333333332</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -564,7 +564,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -572,7 +572,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -581,7 +581,7 @@
       </c>
       <c r="C7" s="3"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -589,7 +589,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -597,7 +597,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -605,7 +605,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -613,7 +613,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -621,7 +621,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -629,7 +629,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -637,7 +637,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -645,7 +645,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>15</v>
       </c>
@@ -653,7 +653,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>16</v>
       </c>
@@ -661,7 +661,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>17</v>
       </c>
@@ -669,7 +669,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>18</v>
       </c>
@@ -677,7 +677,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>19</v>
       </c>
@@ -685,7 +685,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>20</v>
       </c>
@@ -693,7 +693,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>21</v>
       </c>
@@ -701,7 +701,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>22</v>
       </c>
@@ -709,7 +709,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>23</v>
       </c>
@@ -718,7 +718,7 @@
       </c>
       <c r="D24" s="3"/>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>24</v>
       </c>
@@ -726,7 +726,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>25</v>
       </c>
@@ -734,7 +734,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>26</v>
       </c>
@@ -742,7 +742,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>27</v>
       </c>
@@ -750,7 +750,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>28</v>
       </c>
@@ -758,7 +758,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>29</v>
       </c>
@@ -766,12 +766,12 @@
         <v>36</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>